<commit_message>
update Sat 2025-01-04 T-590 part2
</commit_message>
<xml_diff>
--- a/_data/Osmismerky/2025-01_KO/Results/2025-01_KO_results.xlsx
+++ b/_data/Osmismerky/2025-01_KO/Results/2025-01_KO_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git_atlantis\SourceCodes\Lusteni_GitHub\_data\Osmismerky\2025-01_KO\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DBA0CA-B87E-4BCD-840B-D2EB5ECB4327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA681BEA-8EBF-45FC-8C07-51907EE5B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37050" yWindow="975" windowWidth="17280" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37050" yWindow="975" windowWidth="17280" windowHeight="13230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
@@ -2325,9 +2325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D74E096-B76D-4254-90EC-1ACF60B0DC5D}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3695,7 +3695,7 @@
         <v>188</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69:E124" si="3">LEN(C69)</f>
+        <f t="shared" ref="E69:E122" si="3">LEN(C69)</f>
         <v>19</v>
       </c>
       <c r="F69">

</xml_diff>

<commit_message>
update Tue 2025-01-07 T-590 HF
</commit_message>
<xml_diff>
--- a/_data/Osmismerky/2025-01_KO/Results/2025-01_KO_results.xlsx
+++ b/_data/Osmismerky/2025-01_KO/Results/2025-01_KO_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git_atlantis\SourceCodes\Lusteni_GitHub\_data\Osmismerky\2025-01_KO\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA681BEA-8EBF-45FC-8C07-51907EE5B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AEC876-F59B-4731-85B3-C731B8E30173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37050" yWindow="975" windowWidth="17280" windowHeight="13230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="0" windowWidth="17280" windowHeight="12384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="313">
   <si>
     <t>time to solve</t>
   </si>
@@ -953,6 +953,18 @@
   </si>
   <si>
     <t>HAN</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>HNovot</t>
+  </si>
+  <si>
+    <t>HAN, Hnovot</t>
+  </si>
+  <si>
+    <t>PM, Hnovot</t>
   </si>
 </sst>
 </file>
@@ -2326,8 +2338,8 @@
   <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2496,6 +2508,9 @@
       <c r="C9" t="s">
         <v>141</v>
       </c>
+      <c r="D9" t="s">
+        <v>310</v>
+      </c>
       <c r="E9">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2612,7 +2627,7 @@
         <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -2708,7 +2723,7 @@
         <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
@@ -2816,6 +2831,9 @@
       <c r="C25" t="s">
         <v>157</v>
       </c>
+      <c r="D25" t="s">
+        <v>310</v>
+      </c>
       <c r="E25">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2876,7 +2894,7 @@
         <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
@@ -2960,7 +2978,7 @@
         <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
@@ -3134,6 +3152,9 @@
       <c r="C40" t="s">
         <v>168</v>
       </c>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
       <c r="E40">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -3286,6 +3307,9 @@
       <c r="C48" t="s">
         <v>173</v>
       </c>
+      <c r="D48" t="s">
+        <v>312</v>
+      </c>
       <c r="E48">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -3330,6 +3354,9 @@
       <c r="C50" t="s">
         <v>175</v>
       </c>
+      <c r="D50" t="s">
+        <v>309</v>
+      </c>
       <c r="E50">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3374,6 +3401,9 @@
       <c r="C52" t="s">
         <v>177</v>
       </c>
+      <c r="D52" t="s">
+        <v>310</v>
+      </c>
       <c r="E52">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -3396,6 +3426,9 @@
       <c r="C53" t="s">
         <v>178</v>
       </c>
+      <c r="D53" t="s">
+        <v>309</v>
+      </c>
       <c r="E53">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -3467,6 +3500,9 @@
       <c r="C57" t="s">
         <v>180</v>
       </c>
+      <c r="D57" t="s">
+        <v>309</v>
+      </c>
       <c r="E57">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3650,6 +3686,9 @@
       <c r="C67" t="s">
         <v>186</v>
       </c>
+      <c r="D67" t="s">
+        <v>310</v>
+      </c>
       <c r="E67">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -3740,6 +3779,9 @@
       <c r="C72" t="s">
         <v>189</v>
       </c>
+      <c r="D72" t="s">
+        <v>309</v>
+      </c>
       <c r="E72">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -3818,6 +3860,9 @@
       <c r="C76" t="s">
         <v>192</v>
       </c>
+      <c r="D76" t="s">
+        <v>309</v>
+      </c>
       <c r="E76">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -3906,6 +3951,9 @@
       <c r="C80" t="s">
         <v>196</v>
       </c>
+      <c r="D80" t="s">
+        <v>309</v>
+      </c>
       <c r="E80">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -3940,6 +3988,9 @@
       <c r="C82" t="s">
         <v>197</v>
       </c>
+      <c r="D82" t="s">
+        <v>309</v>
+      </c>
       <c r="E82">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -4017,6 +4068,9 @@
       </c>
       <c r="C86" t="s">
         <v>200</v>
+      </c>
+      <c r="D86" t="s">
+        <v>309</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>

</xml_diff>